<commit_message>
conditions-for-access-and-usage: updated xlsx and ttl
</commit_message>
<xml_diff>
--- a/conditions-for-access-and-usage/conditions-for-access-and-usage.xlsx
+++ b/conditions-for-access-and-usage/conditions-for-access-and-usage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabularies\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D638C6-5A3F-4EF1-A9B2-C1FA2E3F8308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3C57D0-14F1-4220-9E9A-182C9F9C2410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -85,9 +85,6 @@
     <t>https://creativecommons.org/licenses/by/4.0/</t>
   </si>
   <si>
-    <t>My comments (not parsed by the tool).</t>
-  </si>
-  <si>
     <t>URI</t>
   </si>
   <si>
@@ -127,10 +124,25 @@
     <t>owl:priorVersion</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>Published Controlled Vocabulary</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/1.0.0</t>
+  </si>
+  <si>
+    <t>Licence provided, free of charge</t>
+  </si>
+  <si>
+    <t>Licence provided, fee required</t>
+  </si>
+  <si>
+    <t>Contractual arrangement, free of charge</t>
+  </si>
+  <si>
+    <t>Contractual arrangement, fee required</t>
   </si>
 </sst>
 </file>
@@ -209,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -229,6 +241,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,7 +551,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -546,23 +559,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="95.140625" customWidth="1"/>
-    <col min="2" max="2" width="74.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="95.109375" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -570,7 +583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -579,7 +592,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -588,7 +601,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -597,7 +610,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -606,7 +619,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -615,19 +628,19 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -636,24 +649,26 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="str">
         <f>_xlfn.CONCAT(B1,"/",B9)</f>
-        <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/1.0.0</v>
+        <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/1.1.0</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -662,107 +677,138 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B19)," ","-"),",",""))</f>
         <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/licence-provided</v>
       </c>
       <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f t="shared" ref="A20:A28" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B20)," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/contractual-arrangement</v>
+      </c>
+      <c r="B20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
-        <f t="shared" ref="A20:A24" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B20)," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/contractual-arrangement</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/free-of-charge</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/fee-required</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/royalty-free</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/licence-provided-free-of-charge</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/licence-provided-fee-required</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/contractual-arrangement-free-of-charge</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/contractual-arrangement-fee-required</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/conditions-for-access-and-usage/other</v>
       </c>
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="8"/>
+    </row>
+    <row r="36" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -781,13 +827,35 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date_x002f_Heure xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
+    <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100156B981FAAFB4349A28B03AB4EEECF9F" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e7c9bb6974a57a0073a8d48fc3b6089">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ea66b1c-fa60-4493-a86c-b420df37761a" xmlns:ns3="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d5753863158ce54f5fdf0d8971fe3971" ns2:_="" ns3:_="">
     <xsd:import namespace="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
@@ -1050,29 +1118,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9660C0FD-9E19-44E9-98F2-CD1ED4F5794F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
+    <ds:schemaRef ds:uri="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date_x002f_Heure xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ea66b1c-fa60-4493-a86c-b420df37761a" xsi:nil="true"/>
-    <note xmlns="322c47a9-7cf9-4f39-ba36-4bf679c08fb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93F42387-0D43-4809-A247-7AAC6E57EA99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1089,23 +1154,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{354E852E-38F4-443F-ABCC-E4BE2043727A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9660C0FD-9E19-44E9-98F2-CD1ED4F5794F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="322c47a9-7cf9-4f39-ba36-4bf679c08fb0"/>
-    <ds:schemaRef ds:uri="4ea66b1c-fa60-4493-a86c-b420df37761a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>